<commit_message>
Fix some errors in scrap retry
</commit_message>
<xml_diff>
--- a/resources/channels.xlsx
+++ b/resources/channels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,22 +766,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Centelha Vermelha</t>
+          <t>Carolline Sardá</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@CentelhaVermelha1917</t>
+          <t>https://www.youtube.com/@CarollineSarda</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Um canal dedicado ao fortalecimento dos nossos camaradas, cortes, videos, traducoes. Siga os canais dos camaradas pelo link na descricao de cada video ou pel...</t>
+          <t xml:space="preserve">Conto historias de mulheres, explico sobre direitos feministas e faco alguns reacts radioativos nas horas vagas. </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>UCQTE34TpHjpkwUBlgcLiecA</t>
+          <t>UCo3oa06jhy5K-G5ytlFbiUg</t>
         </is>
       </c>
     </row>
@@ -791,22 +791,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Centro Socialista</t>
+          <t>Centelha Vermelha</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@centrosocialista1824</t>
+          <t>https://www.youtube.com/@CentelhaVermelha1917</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Canal da Associacao Popular dos Centros Socialistas.</t>
+          <t>Um canal dedicado ao fortalecimento dos nossos camaradas, cortes, videos, traducoes. Siga os canais dos camaradas pelo link na descricao de cada video ou pel...</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>UC4irEnt6IRnrWxBUdCPDf7w</t>
+          <t>UCQTE34TpHjpkwUBlgcLiecA</t>
         </is>
       </c>
     </row>
@@ -816,22 +816,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Chavoso da USP</t>
+          <t>Centro Socialista</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@ChavosodaUSP</t>
+          <t>https://www.youtube.com/@centrosocialista1824</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>"Injetar odio no cerebro do conformado, informacao no desinformado e autoestima no derrotado".-- Faccao Central</t>
+          <t>Canal da Associacao Popular dos Centros Socialistas.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>UCKWus46Vy8gwf1rRLu4II0w</t>
+          <t>UC4irEnt6IRnrWxBUdCPDf7w</t>
         </is>
       </c>
     </row>
@@ -841,22 +841,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cortes do Chocolate</t>
+          <t>Chavoso da USP</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@cortesdochocolate</t>
+          <t>https://www.youtube.com/@ChavosodaUSP</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Cortes da live do Chocolate!</t>
+          <t>"Injetar odio no cerebro do conformado, informacao no desinformado e autoestima no derrotado".-- Faccao Central</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>UCDBogqb0qIhQtLQZ2pWyq2Q</t>
+          <t>UCKWus46Vy8gwf1rRLu4II0w</t>
         </is>
       </c>
     </row>
@@ -866,22 +866,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cortes do História Pública</t>
+          <t>Cortes do Chocolate</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@CortesdoHistoriaPublica</t>
+          <t>https://www.youtube.com/@cortesdochocolate</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Canal de cortes oficial do Historia Publica.</t>
+          <t>Cortes da live do Chocolate!</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>UCAMExYqcweM7PUebKfmLdFA</t>
+          <t>UCDBogqb0qIhQtLQZ2pWyq2Q</t>
         </is>
       </c>
     </row>
@@ -891,22 +891,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cortes do João Carvalho [OFICIAL]</t>
+          <t>Cortes do História Pública</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@CortesdoJoao</t>
+          <t>https://www.youtube.com/@CortesdoHistoriaPublica</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>CANAL OFICIAL de CORTES do Joao Carvalho, que e historiador, mestre, doutorando e professor, dentre outras tantas coisas!Conheca e inscreva-se no canal princ...</t>
+          <t>Canal de cortes oficial do Historia Publica.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>UCawkKjxvsJ1oShKVK4xxfJQ</t>
+          <t>UCAMExYqcweM7PUebKfmLdFA</t>
         </is>
       </c>
     </row>
@@ -916,22 +916,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DESCE A LETRA SHOW</t>
+          <t>Cortes do João Carvalho [OFICIAL]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@DESCEALETRASHOW</t>
+          <t>https://www.youtube.com/@CortesdoJoao</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>CANAL OFICIAL de CORTES do Joao Carvalho, que e historiador, mestre, doutorando e professor, dentre outras tantas coisas!Conheca e inscreva-se no canal princ...</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>UCCD93px0UneWNFg_HxV4naQ</t>
+          <t>UCawkKjxvsJ1oShKVK4xxfJQ</t>
         </is>
       </c>
     </row>
@@ -941,22 +941,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DESCE A LETRA SHOW - CORTES</t>
+          <t>DESCE A LETRA SHOW</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@DESCEALETRASHOWCORTES</t>
+          <t>https://www.youtube.com/@DESCEALETRASHOW</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Canal com os melhores momentos dos episodios diarios e ao vivo do podcast Desce a Letra Show, com Caue Moura e Load Comics na apresentacao trazendo as maiore...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>UCpKYQv-V68npJnHLkZFZZyg</t>
+          <t>UCCD93px0UneWNFg_HxV4naQ</t>
         </is>
       </c>
     </row>
@@ -966,22 +966,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Dan McClellan</t>
+          <t>DESCE A LETRA SHOW - CORTES</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@maklelan</t>
+          <t>https://www.youtube.com/@DESCEALETRASHOWCORTES</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Canal com os melhores momentos dos episodios diarios e ao vivo do podcast Desce a Letra Show, com Caue Moura e Load Comics na apresentacao trazendo as maiore...</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>UCAAJCQ0FCqRmAEv95SyTfNg</t>
+          <t>UCpKYQv-V68npJnHLkZFZZyg</t>
         </is>
       </c>
     </row>
@@ -991,22 +991,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Daniel Duncan</t>
+          <t>Dan McClellan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@DanielDuncan</t>
+          <t>https://www.youtube.com/@maklelan</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.danielduncan.com.br/</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>UCVAHiMT4a8Q-Kny0RRe-Gig</t>
+          <t>UCAAJCQ0FCqRmAEv95SyTfNg</t>
         </is>
       </c>
     </row>
@@ -1016,22 +1016,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Doutora Drag - Dimitra Vulcana</t>
+          <t>Daniel Duncan</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@DoutoraDrag</t>
+          <t>https://www.youtube.com/@DanielDuncan</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>O Doutora Drag e um canal feito pela Dimitra Vulcana, drag queen, professora, doutora em ciencias da saude. A ideia do canal e contribuir com a formacao marx...</t>
+          <t>https://www.danielduncan.com.br/</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>UCcgl8D1QAwAmZekgv1-BaQg</t>
+          <t>UCVAHiMT4a8Q-Kny0RRe-Gig</t>
         </is>
       </c>
     </row>
@@ -1041,22 +1041,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Dudabolche</t>
+          <t>Doutora Drag - Dimitra Vulcana</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@dudabolche3466</t>
+          <t>https://www.youtube.com/@DoutoraDrag</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>O Doutora Drag e um canal feito pela Dimitra Vulcana, drag queen, professora, doutora em ciencias da saude. A ideia do canal e contribuir com a formacao marx...</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>UCjRgkN0Vz5CEkppxvzu5DDA</t>
+          <t>UCcgl8D1QAwAmZekgv1-BaQg</t>
         </is>
       </c>
     </row>
@@ -1066,22 +1066,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Eduardo Moreira</t>
+          <t>Dudabolche</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@EduardoMoreira</t>
+          <t>https://www.youtube.com/@dudabolche3466</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Eduardo Moreira e formado em Engenharia pela PUC RJ e estudou Economia na Universidade da California de San Diego (UCSD), sendo eleito o melhor aluno do curs...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>UC7cIZNwQhE1o8kopShrQHvw</t>
+          <t>UCjRgkN0Vz5CEkppxvzu5DDA</t>
         </is>
       </c>
     </row>
@@ -1091,22 +1091,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Epoch Philosophy</t>
+          <t>Eduardo Moreira</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@epochphilosophy</t>
+          <t>https://www.youtube.com/@EduardoMoreira</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Art, theory, technology, and philosophy.</t>
+          <t>Eduardo Moreira e formado em Engenharia pela PUC RJ e estudou Economia na Universidade da California de San Diego (UCSD), sendo eleito o melhor aluno do curs...</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>UC738SsV6BSLUVvMgKnEFFzQ</t>
+          <t>UC7cIZNwQhE1o8kopShrQHvw</t>
         </is>
       </c>
     </row>
@@ -1116,22 +1116,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Estudos Marxistas</t>
+          <t>Epoch Philosophy</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@EstudosMarxistas</t>
+          <t>https://www.youtube.com/@epochphilosophy</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Art, theory, technology, and philosophy.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>UCeqa-WZyI3gxNQg0cntPW8g</t>
+          <t>UC738SsV6BSLUVvMgKnEFFzQ</t>
         </is>
       </c>
     </row>
@@ -1141,22 +1141,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>F.D Signifier</t>
+          <t>Estudos Marxistas</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@FDSignifire</t>
+          <t>https://www.youtube.com/@EstudosMarxistas</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Come here to watch my video essays on black movies and media</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>UCgi2u-lGY-2i2ubLsUr6FbQ</t>
+          <t>UCeqa-WZyI3gxNQg0cntPW8g</t>
         </is>
       </c>
     </row>
@@ -1166,22 +1166,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>First Thought</t>
+          <t>F.D Signifier</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@firstthoughtnews</t>
+          <t>https://www.youtube.com/@FDSignifire</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Biased news. Three times a week.</t>
+          <t>Come here to watch my video essays on black movies and media</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>UCb5CyUGW_tODKqsOknphG-A</t>
+          <t>UCgi2u-lGY-2i2ubLsUr6FbQ</t>
         </is>
       </c>
     </row>
@@ -1191,22 +1191,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fredda</t>
+          <t>First Thought</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@FreddaYT</t>
+          <t>https://www.youtube.com/@firstthoughtnews</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Sponsorship inquiries: freddabusiness@gmail.comHistory &amp; Gaming. I've got a degree in history that I try to leverage to provide insightful content where I do...</t>
+          <t>Biased news. Three times a week.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>UCrbPsI5RvQybygZykPUxBSA</t>
+          <t>UCb5CyUGW_tODKqsOknphG-A</t>
         </is>
       </c>
     </row>
@@ -1216,22 +1216,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fábio L. Stern - Ciência da Religião</t>
+          <t>Fredda</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@cienciadareligiao</t>
+          <t>https://www.youtube.com/@FreddaYT</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Canal sobre o estudo cientifico das religioes, com debates de interesse sobre minhas pesquisas, congressos e assuntos gerais da minha vida profissional acade...</t>
+          <t>Sponsorship inquiries: freddabusiness@gmail.comHistory &amp; Gaming. I've got a degree in history that I try to leverage to provide insightful content where I do...</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>UCt_1rDKo7pTAg4pcNZ2G-_Q</t>
+          <t>UCrbPsI5RvQybygZykPUxBSA</t>
         </is>
       </c>
     </row>
@@ -1241,22 +1241,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>GDF</t>
+          <t>Froggy Oficial</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@GDFofficial</t>
+          <t>https://www.youtube.com/channel/UCjKQY7MtCDUsy6v6D1Ed7hg</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Ola! Me chamo Lucas, mas pode me chamar de froggy, sapo, e outras variacoes! Aqui voce vai encontrar conteudo de  seguranca da informacao, tecnologia e princ...</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>UCylNpQCufmDdAhs8CdLmUXQ</t>
+          <t>UCjKQY7MtCDUsy6v6D1Ed7hg</t>
         </is>
       </c>
     </row>
@@ -1266,22 +1266,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Galãs Feios</t>
+          <t>Fábio L. Stern - Ciência da Religião</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@GalasFeios</t>
+          <t>https://www.youtube.com/@cienciadareligiao</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Humor e opiniao sobre politica e cultura pop em geral pelos amigos Helder Maldonado e Marco Bezzi, que destilam seu odio festivo pra falar tambem de musica, ...</t>
+          <t>Canal sobre o estudo cientifico das religioes, com debates de interesse sobre minhas pesquisas, congressos e assuntos gerais da minha vida profissional acade...</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>UC2bZgihqibFD_vhaYEXQZFg</t>
+          <t>UCt_1rDKo7pTAg4pcNZ2G-_Q</t>
         </is>
       </c>
     </row>
@@ -1291,22 +1291,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Grupo de Estudos 9 de Maio</t>
+          <t>GDF</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@GrupodeEstudos9deMaio</t>
+          <t>https://www.youtube.com/@GDFofficial</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>O Grupo de Estudos 9 de Maio e destinado ao estudo da Segunda Guerra Mundial na Uniao Sovietica e no Brasil.</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>UCGpGmfuZJcXVqFg59-qJUiQ</t>
+          <t>UCylNpQCufmDdAhs8CdLmUXQ</t>
         </is>
       </c>
     </row>
@@ -1316,22 +1316,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Guerra Patriótica</t>
+          <t>Galãs Feios</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@GuerraPatrioticaEstudos</t>
+          <t>https://www.youtube.com/@GalasFeios</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>O canal destina-se a analisar e debater os eventos politicos do Brasil e do mundo.A Segunda Guerra Mundial, com enfase na Frete Leste, tratando o periodo com...</t>
+          <t>Humor e opiniao sobre politica e cultura pop em geral pelos amigos Helder Maldonado e Marco Bezzi, que destilam seu odio festivo pra falar tambem de musica, ...</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>UCO7xOICU0tWtQgEuDkCugYw</t>
+          <t>UC2bZgihqibFD_vhaYEXQZFg</t>
         </is>
       </c>
     </row>
@@ -1341,22 +1341,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Hakim</t>
+          <t>Grupo de Estudos 9 de Maio</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@YaBoiHakim</t>
+          <t>https://www.youtube.com/@GrupodeEstudos9deMaio</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>la ilha ilaW 'llh Some guy that makes videos from time to time.Patreon: https://www.patreon.com/ComradeHakimTwitter: https://twitter.com/YaBoiHakim</t>
+          <t>O Grupo de Estudos 9 de Maio e destinado ao estudo da Segunda Guerra Mundial na Uniao Sovietica e no Brasil.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>UCPPZoYsfoSekIpLcz9plX1Q</t>
+          <t>UCGpGmfuZJcXVqFg59-qJUiQ</t>
         </is>
       </c>
     </row>
@@ -1366,22 +1366,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Heribaldo Maia</t>
+          <t>Guerra Patriótica</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@heribaldomaia</t>
+          <t>https://www.youtube.com/@GuerraPatrioticaEstudos</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Canal de educacao que visa ajudar na formacao politica e teorica por uma perspectiva critica. Simbora?.QUEM SOU EU?Sou formado em Historia e mestrando em fil...</t>
+          <t>O canal destina-se a analisar e debater os eventos politicos do Brasil e do mundo.A Segunda Guerra Mundial, com enfase na Frete Leste, tratando o periodo com...</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>UCr2isBDXfD01ZEw7EEzcLCg</t>
+          <t>UCO7xOICU0tWtQgEuDkCugYw</t>
         </is>
       </c>
     </row>
@@ -1391,22 +1391,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>História Cabeluda</t>
+          <t>Hakim</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@HistoriaCabeluda</t>
+          <t>https://www.youtube.com/@YaBoiHakim</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Canal que produz e publica materiais voltados para a educacao politica dos trabalhadores para construir a Revolucao Brasileira. </t>
+          <t>la ilha ilaW 'llh Some guy that makes videos from time to time.Patreon: https://www.patreon.com/ComradeHakimTwitter: https://twitter.com/YaBoiHakim</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>UCqbz_4hrf2D58UFBOleuFnQ</t>
+          <t>UCPPZoYsfoSekIpLcz9plX1Q</t>
         </is>
       </c>
     </row>
@@ -1416,22 +1416,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>História Pública</t>
+          <t>Heribaldo Maia</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@HistoriaPublicaOficial</t>
+          <t>https://www.youtube.com/@heribaldomaia</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Um canal dedicado a informacao, ao debate e a analise politica feito por historiadores marxistas.</t>
+          <t>Canal de educacao que visa ajudar na formacao politica e teorica por uma perspectiva critica. Simbora?.QUEM SOU EU?Sou formado em Historia e mestrando em fil...</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>UCcoxGCRGcq6FhHbEvr2y9Vg</t>
+          <t>UCr2isBDXfD01ZEw7EEzcLCg</t>
         </is>
       </c>
     </row>
@@ -1441,22 +1441,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Humberto Matos</t>
+          <t>Historiatopia</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@HumbertoMatos</t>
+          <t>https://www.youtube.com/@lorquisa1</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Canal de criticas sobre economia politica com pitadas de historia, filosofia e sociologia.Seja um dos nossos apoiadores e ajude a manter o Canal:Nosso site c...</t>
+          <t xml:space="preserve">Historiador, comunicador, podcaster, streamer e professor. </t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>UC3qAUf53j_dUv09jH7jsUJw</t>
+          <t>UCfWFv2KvdZ5Gq_mTvcdgQRA</t>
         </is>
       </c>
     </row>
@@ -1466,22 +1466,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ICL NOTICIAS CORTES [OFICIAL]</t>
+          <t>História Cabeluda</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@iclnoticias</t>
+          <t>https://www.youtube.com/@HistoriaCabeluda</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> | Canal oficial de cortes do ICL Noticias. Aqui voce encontra os trechos das principais noticias e debates da sociedade brasileira.  Faca parte do Insti...</t>
+          <t xml:space="preserve">Canal que produz e publica materiais voltados para a educacao politica dos trabalhadores para construir a Revolucao Brasileira. </t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>UCTnRtQ9IkBGmCKcLB31BcyA</t>
+          <t>UCqbz_4hrf2D58UFBOleuFnQ</t>
         </is>
       </c>
     </row>
@@ -1491,22 +1491,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Instituto Conhecimento Liberta</t>
+          <t>História Pública</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@InstitutoConhecimentoLiberta</t>
+          <t>https://www.youtube.com/@HistoriaPublicaOficial</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>O Instituto Conhecimento Liberta e uma empresa de jornalismo e educacao com noticiarios digitais diarios. Nossa programacao inclui noticiarios, podcasts e pr...</t>
+          <t>Um canal dedicado a informacao, ao debate e a analise politica feito por historiadores marxistas.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>UCaIqJHHo9TJiLINzOFJRl2Q</t>
+          <t>UCcoxGCRGcq6FhHbEvr2y9Vg</t>
         </is>
       </c>
     </row>
@@ -1516,22 +1516,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ismeiow</t>
+          <t>Humberto Matos</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Ismeiow</t>
+          <t>https://www.youtube.com/@HumbertoMatos</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Hey eu sou a Ismeiow, e aqui voce vai encontrar uma drag queen tentando te fazer rir, nem que seja de odio</t>
+          <t>Canal de criticas sobre economia politica com pitadas de historia, filosofia e sociologia.Seja um dos nossos apoiadores e ajude a manter o Canal:Nosso site c...</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>UCnmBz-89n3pIpQXqcrWCv_g</t>
+          <t>UC3qAUf53j_dUv09jH7jsUJw</t>
         </is>
       </c>
     </row>
@@ -1541,22 +1541,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>JohntheDuncan</t>
+          <t>ICL NOTICIAS CORTES [OFICIAL]</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@JohntheDuncan</t>
+          <t>https://www.youtube.com/@iclnoticias</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PhD researcher in Human Rights, austerity and neoliberalism |Disco Socialist trying to YouTube Patreon | https://www.patreon.com/johntheduncan| Twitter: http...</t>
+          <t xml:space="preserve"> | Canal oficial de cortes do ICL Noticias. Aqui voce encontra os trechos das principais noticias e debates da sociedade brasileira.  Faca parte do Insti...</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>UCjZNuiHWaxFhtaI1EAlSXlg</t>
+          <t>UCTnRtQ9IkBGmCKcLB31BcyA</t>
         </is>
       </c>
     </row>
@@ -1566,22 +1566,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Jonas Čeika - CCK Philosophy</t>
+          <t>Instituto Conhecimento Liberta</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@jonasceikaCCK</t>
+          <t>https://www.youtube.com/@InstitutoConhecimentoLiberta</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>I make videos on philosophy, politics, and cultural theory.My book on Marx and Nietzsche - How to Philosophize with a Hammer and Sickle - is available for pr...</t>
+          <t>O Instituto Conhecimento Liberta e uma empresa de jornalismo e educacao com noticiarios digitais diarios. Nossa programacao inclui noticiarios, podcasts e pr...</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>UCSkzHxIcfoEr69MWBdo0ppg</t>
+          <t>UCaIqJHHo9TJiLINzOFJRl2Q</t>
         </is>
       </c>
     </row>
@@ -1591,22 +1591,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Jones Manoel</t>
+          <t>Ismeiow</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@JonesManoel</t>
+          <t>https://www.youtube.com/@Ismeiow</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Hey eu sou a Ismeiow, e aqui voce vai encontrar uma drag queen tentando te fazer rir, nem que seja de odio</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>UC02coXfDPjEmU8uDT2G8Z2A</t>
+          <t>UCnmBz-89n3pIpQXqcrWCv_g</t>
         </is>
       </c>
     </row>
@@ -1616,22 +1616,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Jornal A Verdade</t>
+          <t>JohntheDuncan</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@JornalAVerdadetv</t>
+          <t>https://www.youtube.com/@JohntheDuncan</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Um jornal dos trabalhadores na luta pelo Socialismo.Leia, Assine e Divulgue o Jornal A Verdade!http://averdade.org.br/assinatura/</t>
+          <t>PhD researcher in Human Rights, austerity and neoliberalism |Disco Socialist trying to YouTube Patreon | https://www.patreon.com/johntheduncan| Twitter: http...</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>UCd4U49PdTyEY2e2QKR6StZg</t>
+          <t>UCjZNuiHWaxFhtaI1EAlSXlg</t>
         </is>
       </c>
     </row>
@@ -1641,22 +1641,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>João Carvalho</t>
+          <t>Jonas Čeika - CCK Philosophy</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@assimdisseojoao</t>
+          <t>https://www.youtube.com/@jonasceikaCCK</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Historiador e militante comunista. MLM. Youtuber e Streamer no /assimdisseojoaoMembro do coletivo SoberanaRebelar-se e justo!Conheca tambem o canal de cortes...</t>
+          <t>I make videos on philosophy, politics, and cultural theory.My book on Marx and Nietzsche - How to Philosophize with a Hammer and Sickle - is available for pr...</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>UC7-Pp09PJX_SYP9oyMzUAtg</t>
+          <t>UCSkzHxIcfoEr69MWBdo0ppg</t>
         </is>
       </c>
     </row>
@@ -1666,22 +1666,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ju Furno</t>
+          <t>Jones Manoel</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@JuFurno</t>
+          <t>https://www.youtube.com/@JonesManoel</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>@JuFurno e uma mulher jovem. E gaucha, torce para o colorado mas vive em sampa. E mestre e doutora em desenvolvimento economico no instituto de economia da u...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>UCQNp5qrzckO45QFyaVPh9Lg</t>
+          <t>UC02coXfDPjEmU8uDT2G8Z2A</t>
         </is>
       </c>
     </row>
@@ -1691,22 +1691,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Justificando</t>
+          <t>Jornal A Verdade</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Justificando</t>
+          <t>https://www.youtube.com/@JornalAVerdadetv</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Inscreva-se no canal do Justificando no Youtube. | Mentes inquietas, pensam direito.</t>
+          <t>Um jornal dos trabalhadores na luta pelo Socialismo.Leia, Assine e Divulgue o Jornal A Verdade!http://averdade.org.br/assinatura/</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>UClGI_T5ZXjHNBbpKrERbFHQ</t>
+          <t>UCd4U49PdTyEY2e2QKR6StZg</t>
         </is>
       </c>
     </row>
@@ -1716,22 +1716,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Kathrin</t>
+          <t>João Carvalho</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Kathrin_yt</t>
+          <t>https://www.youtube.com/@assimdisseojoao</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Welding our outward political/social revolutions, with deep inner reflection and evolution of our consciousness.  </t>
+          <t>Historiador e militante comunista. MLM. Youtuber e Streamer no /assimdisseojoaoMembro do coletivo SoberanaRebelar-se e justo!Conheca tambem o canal de cortes...</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>UCVbWFrI5NrLCWIjjW5cbzMg</t>
+          <t>UC7-Pp09PJX_SYP9oyMzUAtg</t>
         </is>
       </c>
     </row>
@@ -1741,22 +1741,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Kultura Kritica</t>
+          <t>Ju Furno</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@kulturakritica</t>
+          <t>https://www.youtube.com/@JuFurno</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Me chamo Koba e sou estudante de Historia e Historia da Arte e busco trazer de forma didatica conteudo sobre historia da arte e suas relacoes com a politica ...</t>
+          <t>@JuFurno e uma mulher jovem. E gaucha, torce para o colorado mas vive em sampa. E mestre e doutora em desenvolvimento economico no instituto de economia da u...</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>UCjUENpzJWtzcF47BGE29A7w</t>
+          <t>UCQNp5qrzckO45QFyaVPh9Lg</t>
         </is>
       </c>
     </row>
@@ -1766,22 +1766,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Lady Izdihar</t>
+          <t>Justificando</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@LadyIzdihar</t>
+          <t>https://www.youtube.com/@Justificando</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Asalam alaikum comrades!I'm a historian on Russian history but mostly focus on the first 30-40 years and the cultural and ethnographic makeup of what the USS...</t>
+          <t>Inscreva-se no canal do Justificando no Youtube. | Mentes inquietas, pensam direito.</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>UCgCeGl_P4ldTcpHNCC-6Nfw</t>
+          <t>UClGI_T5ZXjHNBbpKrERbFHQ</t>
         </is>
       </c>
     </row>
@@ -1791,22 +1791,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Laura Sabino</t>
+          <t>Kathrin</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@mylaura_m</t>
+          <t>https://www.youtube.com/@Kathrin_yt</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t xml:space="preserve">Welding our outward political/social revolutions, with deep inner reflection and evolution of our consciousness.  </t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>UCCmh3nJayT-7jEM6hg2vP9Q</t>
+          <t>UCVbWFrI5NrLCWIjjW5cbzMg</t>
         </is>
       </c>
     </row>
@@ -1816,22 +1816,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Leandro Demori</t>
+          <t>Kultura Kritica</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@leandrodemori</t>
+          <t>https://www.youtube.com/@kulturakritica</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Ola, este e o meu canal ------------# Voce pode assinar GRATIS a minha newsletter # + copie e cole o link abaixo no seu navegador +                  www.agr...</t>
+          <t>Me chamo Koba e sou estudante de Historia e Historia da Arte e busco trazer de forma didatica conteudo sobre historia da arte e suas relacoes com a politica ...</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>UCKvo5P4W0tNYAWORXEqEp-Q</t>
+          <t>UCjUENpzJWtzcF47BGE29A7w</t>
         </is>
       </c>
     </row>
@@ -1841,22 +1841,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>LucasZawacki</t>
+          <t>Lady Izdihar</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@LucasZawacki</t>
+          <t>https://www.youtube.com/@LadyIzdihar</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Free Software, games and music</t>
+          <t>Asalam alaikum comrades!I'm a historian on Russian history but mostly focus on the first 30-40 years and the cultural and ethnographic makeup of what the USS...</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>UCaLneog2uRaLcOHFAP6QD5A</t>
+          <t>UCgCeGl_P4ldTcpHNCC-6Nfw</t>
         </is>
       </c>
     </row>
@@ -1866,22 +1866,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Marxism Today</t>
+          <t>Laura Sabino</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Marxism_Today</t>
+          <t>https://www.youtube.com/@mylaura_m</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Left-wing political content from a modern Marxist perspective.Hosted by Kasamang Anna and Paul Connolly.Contact us: marxismtodaymedia@gmail.com</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>UCpBRZBzWQ_cCc_9zKG08L-g</t>
+          <t>UCCmh3nJayT-7jEM6hg2vP9Q</t>
         </is>
       </c>
     </row>
@@ -1891,22 +1891,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Marxist-Leninist Theory</t>
+          <t>Leandro Demori</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@marxist-leninisttheory8023</t>
+          <t>https://www.youtube.com/@leandrodemori</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>The channel presents Marxist-Leninist theory in audio book form. Feel free to share the videos on this channel, debate and ask questions.Mostly classics by M...</t>
+          <t>Ola, este e o meu canal ------------# Voce pode assinar GRATIS a minha newsletter # + copie e cole o link abaixo no seu navegador +                  www.agr...</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>UCEzvnHqlIPv0QbXpdoH0f0Q</t>
+          <t>UCKvo5P4W0tNYAWORXEqEp-Q</t>
         </is>
       </c>
     </row>
@@ -1916,22 +1916,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Meteoro Brasil</t>
+          <t>LucasZawacki</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@MeteoroBrasil</t>
+          <t>https://www.youtube.com/@LucasZawacki</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Meteoro e um canal sobre noticias, cultura pop, ciencia e filosofia. Nossa abordagem e critica e nosso trabalho e diligente.Caixa Postal:17905CEP: 80410-981</t>
+          <t>Free Software, games and music</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>UCk5BcU1rOy6hepflk7_q_Pw</t>
+          <t>UCaLneog2uRaLcOHFAP6QD5A</t>
         </is>
       </c>
     </row>
@@ -1941,22 +1941,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Mexie</t>
+          <t>LucasZawacki</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Mexie</t>
+          <t>https://www.youtube.com/@LucasZawacki</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>political economy * environment * liberation</t>
+          <t>Free Software, games and music</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>UCepkun0sH16b-mqxBN22ogA</t>
+          <t>UCaLneog2uRaLcOHFAP6QD5A</t>
         </is>
       </c>
     </row>
@@ -1966,22 +1966,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Miguel Faria</t>
+          <t>Marxism Today</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@MiguelFaria96</t>
+          <t>https://www.youtube.com/@Marxism_Today</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Um canal essencialmente de politica, mas sem perder a javardice. Sobre mim:Mestre em Ciencia Politica pela EEG - Uminho;Licenciado em Administracao Publica p...</t>
+          <t>Left-wing political content from a modern Marxist perspective.Hosted by Kasamang Anna and Paul Connolly.Contact us: marxismtodaymedia@gmail.com</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>UC9FTIof4MZfXcb6sgRWnXWw</t>
+          <t>UCpBRZBzWQ_cCc_9zKG08L-g</t>
         </is>
       </c>
     </row>
@@ -1991,22 +1991,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Minha Aula É Um Show</t>
+          <t>Marxist-Leninist Theory</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@minhaaulaeumshow2951</t>
+          <t>https://www.youtube.com/@marxist-leninisttheory8023</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>O que acontece quando um professoator de filosofisica resolve vir pro youtube?Vem com o tio Foca que voce descobre.</t>
+          <t>The channel presents Marxist-Leninist theory in audio book form. Feel free to share the videos on this channel, debate and ask questions.Mostly classics by M...</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>UCYL1Dq24eDRebdTCzM3fAQg</t>
+          <t>UCEzvnHqlIPv0QbXpdoH0f0Q</t>
         </is>
       </c>
     </row>
@@ -2016,22 +2016,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>NORMOSE</t>
+          <t>Meteoro Brasil</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Normose_</t>
+          <t>https://www.youtube.com/@MeteoroBrasil</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Normose e um canal de brainstorms para quem busca reflexao e conhecimento critico:Historia, Filosofia, Divulgacao cientifica, Politica, Arte e Estetica. Insc...</t>
+          <t>Meteoro e um canal sobre noticias, cultura pop, ciencia e filosofia. Nossa abordagem e critica e nosso trabalho e diligente.Caixa Postal:17905CEP: 80410-981</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>UCqBY-VQ2BxHOWnVpuC7swrw</t>
+          <t>UCk5BcU1rOy6hepflk7_q_Pw</t>
         </is>
       </c>
     </row>
@@ -2041,22 +2041,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>NonCompete</t>
+          <t>Mexie</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@NonCompete</t>
+          <t>https://www.youtube.com/@Mexie</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Non-Compete is a content collective creating educational and entertainment contact from a radical leftist perspective. Every week, our team brings you a line...</t>
+          <t>political economy * environment * liberation</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>UCkZFKKK-0YB0FvwoS8P7nHg</t>
+          <t>UCepkun0sH16b-mqxBN22ogA</t>
         </is>
       </c>
     </row>
@@ -2066,22 +2066,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Not Just Bikes</t>
+          <t>Miguel Faria</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@NotJustBikes</t>
+          <t>https://www.youtube.com/@MiguelFaria96</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Stories of great urban planning and urban experiences from the Netherlands and beyond. There are a lot of reasons why Dutch cities are so great; it's not jus...</t>
+          <t>Um canal essencialmente de politica, mas sem perder a javardice. Sobre mim:Mestre em Ciencia Politica pela EEG - Uminho;Licenciado em Administracao Publica p...</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>UC0intLFzLaudFG-xAvUEO-A</t>
+          <t>UC9FTIof4MZfXcb6sgRWnXWw</t>
         </is>
       </c>
     </row>
@@ -2091,22 +2091,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Opera Mundi</t>
+          <t>Minha Aula É Um Show</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@omundi</t>
+          <t>https://www.youtube.com/@minhaaulaeumshow2951</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Noticias, reportagens especiais e analises criticas sobre os principais acontecimentos do mundo. Fundado em 2008, Opera Mundi informa sobre o mundo a partir ...</t>
+          <t>O que acontece quando um professoator de filosofisica resolve vir pro youtube?Vem com o tio Foca que voce descobre.</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>UCOjUlJ4EpPxuhtT0zEVw25A</t>
+          <t>UCYL1Dq24eDRebdTCzM3fAQg</t>
         </is>
       </c>
     </row>
@@ -2116,22 +2116,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Our Changing Climate</t>
+          <t>NORMOSE</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@OurChangingClimate</t>
+          <t>https://www.youtube.com/@Normose_</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Video essays on a burning planet.</t>
+          <t>Normose e um canal de brainstorms para quem busca reflexao e conhecimento critico:Historia, Filosofia, Divulgacao cientifica, Politica, Arte e Estetica. Insc...</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>UCNXvxXpDJXp-mZu3pFMzYHQ</t>
+          <t>UCqBY-VQ2BxHOWnVpuC7swrw</t>
         </is>
       </c>
     </row>
@@ -2141,22 +2141,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>PCB - Reconstrução Revolucionária</t>
+          <t>NonCompete</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@PCB-RR</t>
+          <t>https://www.youtube.com/@NonCompete</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Non-Compete is a content collective creating educational and entertainment contact from a radical leftist perspective. Every week, our team brings you a line...</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>UCyqtnzqG4JNrXZ6LZjz3cjQ</t>
+          <t>UCkZFKKK-0YB0FvwoS8P7nHg</t>
         </is>
       </c>
     </row>
@@ -2166,22 +2166,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pedagolitica </t>
+          <t>Not Just Bikes</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Pedagolitica</t>
+          <t>https://www.youtube.com/@NotJustBikes</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Stories of great urban planning and urban experiences from the Netherlands and beyond. There are a lot of reasons why Dutch cities are so great; it's not jus...</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>UCWFiaT31JopFSbaXKtb8f-w</t>
+          <t>UC0intLFzLaudFG-xAvUEO-A</t>
         </is>
       </c>
     </row>
@@ -2191,22 +2191,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Philippe Leão</t>
+          <t>Opera Mundi</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@profphilippeleao</t>
+          <t>https://www.youtube.com/@omundi</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Noticias, reportagens especiais e analises criticas sobre os principais acontecimentos do mundo. Fundado em 2008, Opera Mundi informa sobre o mundo a partir ...</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>UCqei9e_PWhja9uopl7mhQNw</t>
+          <t>UCOjUlJ4EpPxuhtT0zEVw25A</t>
         </is>
       </c>
     </row>
@@ -2216,22 +2216,22 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Philippe Leão</t>
+          <t>Our Changing Climate</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@profphilippeleao</t>
+          <t>https://www.youtube.com/@OurChangingClimate</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Video essays on a burning planet.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>UCqei9e_PWhja9uopl7mhQNw</t>
+          <t>UCNXvxXpDJXp-mZu3pFMzYHQ</t>
         </is>
       </c>
     </row>
@@ -2241,22 +2241,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Philosophy Tube</t>
+          <t>PCB - Reconstrução Revolucionária</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@PhilosophyTube</t>
+          <t>https://www.youtube.com/@PCB-RR</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>I'm giving away a philosophy degree for free! Subscribe to learn and boost your brain power!</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>UC2PA-AKmVpU6NKCGtZq_rKQ</t>
+          <t>UCyqtnzqG4JNrXZ6LZjz3cjQ</t>
         </is>
       </c>
     </row>
@@ -2266,22 +2266,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Politics in Command</t>
+          <t xml:space="preserve">Pedagolitica </t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@PoliticsinCommand</t>
+          <t>https://www.youtube.com/@Pedagolitica</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Politics In Command is a source for learning about revolutionary politics, history and theory. </t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>UCqXmdo68uAVMNLRPS5YMd8w</t>
+          <t>UCWFiaT31JopFSbaXKtb8f-w</t>
         </is>
       </c>
     </row>
@@ -2291,22 +2291,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Prof. Basilio Historiando</t>
+          <t>Philippe Leão</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@ProfBasilioHistoriando</t>
+          <t>https://www.youtube.com/@profphilippeleao</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Canal de video-aulas sobre Historia e Humanidades.Uma forma descontraida e critica de se preparar para o vestibular, se ligando nos principais conteudos e co...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>UCnU_8ovaM-lltVmXGY9JPUw</t>
+          <t>UCqei9e_PWhja9uopl7mhQNw</t>
         </is>
       </c>
     </row>
@@ -2316,22 +2316,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Prolekult</t>
+          <t>Philippe Leão</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Prolekult</t>
+          <t>https://www.youtube.com/@profphilippeleao</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Prolekult is a Marxist film, writing and culture platform based in England. The purpose of the project is to provide high-quality film content looking at wor...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>UCEBbylt9Rax3nOP_hyPnMPA</t>
+          <t>UCqei9e_PWhja9uopl7mhQNw</t>
         </is>
       </c>
     </row>
@@ -2341,22 +2341,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Rethinking Marxism</t>
+          <t>Philosophy Tube</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@rethinkingmarxism1719</t>
+          <t>https://www.youtube.com/@PhilosophyTube</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Rethinking Marxism is a peer-reviewed journal produced by the Association for Economic and Social Analysis and published by Routledge/Taylor &amp; Francis. http:...</t>
+          <t>I'm giving away a philosophy degree for free! Subscribe to learn and boost your brain power!</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>UCGHstZ8BEUliSH5C6cij70Q</t>
+          <t>UC2PA-AKmVpU6NKCGtZq_rKQ</t>
         </is>
       </c>
     </row>
@@ -2366,22 +2366,22 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Revista Opera</t>
+          <t>Politics in Command</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@RevistaOpera</t>
+          <t>https://www.youtube.com/@PoliticsinCommand</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>http://www.revistaopera.comA Revista Opera e uma plataforma midiatica independente de esquerda fundada em 11 de abril de 2012.Nos acompanhe tambem pelo Faceb...</t>
+          <t xml:space="preserve">Politics In Command is a source for learning about revolutionary politics, history and theory. </t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>UCZenHSRlcyhYxc-KXKiF9_g</t>
+          <t>UCqXmdo68uAVMNLRPS5YMd8w</t>
         </is>
       </c>
     </row>
@@ -2391,22 +2391,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Revolushow ™</t>
+          <t>Prof. Basilio Historiando</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@RevolushowTM</t>
+          <t>https://www.youtube.com/@ProfBasilioHistoriando</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Irreverencia, socialismo e tudo que ha de bom na esquerda.Estes foram os ingredientes escolhidos para criar um podcast esquerdaralho.Mas o professor Karl Mar...</t>
+          <t>Canal de video-aulas sobre Historia e Humanidades.Uma forma descontraida e critica de se preparar para o vestibular, se ligando nos principais conteudos e co...</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>UCag6nJdH24c2LHRvebYJwRQ</t>
+          <t>UCnU_8ovaM-lltVmXGY9JPUw</t>
         </is>
       </c>
     </row>
@@ -2416,22 +2416,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>RichardDWolff</t>
+          <t>Prolekult</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@RichardDWolff</t>
+          <t>https://www.youtube.com/@Prolekult</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>A lifelong professor of economics, Richard D. Wolff is a well-known critic of contemporary capitalism and the leading proponent of an alternative economic sy...</t>
+          <t>Prolekult is a Marxist film, writing and culture platform based in England. The purpose of the project is to provide high-quality film content looking at wor...</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>UCB-5u8VgFc_TI1aAj8_SmDA</t>
+          <t>UCEBbylt9Rax3nOP_hyPnMPA</t>
         </is>
       </c>
     </row>
@@ -2441,22 +2441,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Second Thought</t>
+          <t>Radio Guerrilha</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@SecondThought</t>
+          <t>https://www.youtube.com/@radioguerrilhaoficial</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Second Thought is a channel devoted to education and analysis of current events from a Socialist perspective. Welcome!SUBSCRIBE HERE: http://bit.ly/2nFsvTSNe...</t>
+          <t>Canal oficial da Radio Guerrilha!Para mais informacoes acessem: twitch.tv/radioguerrilha</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>UCJm2TgUqtK1_NLBrjNQ1P-w</t>
+          <t>UCJ31O21f5N0yiMfbAoHFkBQ</t>
         </is>
       </c>
     </row>
@@ -2466,22 +2466,22 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Senso Comuna</t>
+          <t>Rethinking Marxism</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@SensoComunaivandourado</t>
+          <t>https://www.youtube.com/@rethinkingmarxism1719</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>O canal senso comuna e um espaco onde se encontram pessoas que buscam MicroRevolucoes cotidianas, outras mentes abertas e de humanizacao com base cientifica....</t>
+          <t>Rethinking Marxism is a peer-reviewed journal produced by the Association for Economic and Social Analysis and published by Routledge/Taylor &amp; Francis. http:...</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>UCyJYZugIbTwCx965dZ47aCg</t>
+          <t>UCGHstZ8BEUliSH5C6cij70Q</t>
         </is>
       </c>
     </row>
@@ -2491,22 +2491,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Silvio Almeida</t>
+          <t>Revista Opera</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@silviolual</t>
+          <t>https://www.youtube.com/@RevistaOpera</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Sejam bem vindos ao meu canal!Uma voz ativa e relevante, que ja marca presenca nas redes sociais.Pode chegar que aqui nos vamos falar de assuntos densos atra...</t>
+          <t>http://www.revistaopera.comA Revista Opera e uma plataforma midiatica independente de esquerda fundada em 11 de abril de 2012.Nos acompanhe tambem pelo Faceb...</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>UCW3nde-8K-5BaHAmQLZ7ycg</t>
+          <t>UCZenHSRlcyhYxc-KXKiF9_g</t>
         </is>
       </c>
     </row>
@@ -2516,22 +2516,22 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Soberana</t>
+          <t>Revolushow ™</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@Soberana_TV</t>
+          <t>https://www.youtube.com/@RevolushowTM</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Bem vindo(a) a Soberana!Somos um coletivo de criadores marxistas-leninistas dedicados a producao de conteudo para a internet. Nosso objetivo e ocupar a inter...</t>
+          <t>Irreverencia, socialismo e tudo que ha de bom na esquerda.Estes foram os ingredientes escolhidos para criar um podcast esquerdaralho.Mas o professor Karl Mar...</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>UC8tnKW-FN6LdvKazw5RmOOQ</t>
+          <t>UCag6nJdH24c2LHRvebYJwRQ</t>
         </is>
       </c>
     </row>
@@ -2541,22 +2541,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Socialism For All / S4A ☭ Intensify Class Struggle</t>
+          <t>RichardDWolff</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@SocialismForAll</t>
+          <t>https://www.youtube.com/@RichardDWolff</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>I'm a US American studying Marxism (anti-revisionist Marxism-Leninism).I often post human-read audiobooks of socialist texts, &amp; I organize them into playlist...</t>
+          <t>A lifelong professor of economics, Richard D. Wolff is a well-known critic of contemporary capitalism and the leading proponent of an alternative economic sy...</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>UC5GYwuvmAD_VyV6w5aFnnUw</t>
+          <t>UCB-5u8VgFc_TI1aAj8_SmDA</t>
         </is>
       </c>
     </row>
@@ -2566,22 +2566,22 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Spooky Scary Socialist</t>
+          <t>Second Thought</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@SpookyScarySocialist</t>
+          <t>https://www.youtube.com/@SecondThought</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>eCommunist Homo~Animator</t>
+          <t>Second Thought is a channel devoted to education and analysis of current events from a Socialist perspective. Welcome!SUBSCRIBE HERE: http://bit.ly/2nFsvTSNe...</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>UCl_A_42M6kvjH8Gr-rwfCUw</t>
+          <t>UCJm2TgUqtK1_NLBrjNQ1P-w</t>
         </is>
       </c>
     </row>
@@ -2591,22 +2591,22 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>TV Boitempo</t>
+          <t>Senso Comuna</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TVBoitempo</t>
+          <t>https://www.youtube.com/@SensoComunaivandourado</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Canal de videos da maior editora do pensamento critico da lingua portuguesa, com catalogo consistente reconhecido por sua qualidade e clareza de opcoes edito...</t>
+          <t>O canal senso comuna e um espaco onde se encontram pessoas que buscam MicroRevolucoes cotidianas, outras mentes abertas e de humanizacao com base cientifica....</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>UCzwfw0utuEVxc4D6ggXcqiQ</t>
+          <t>UCyJYZugIbTwCx965dZ47aCg</t>
         </is>
       </c>
     </row>
@@ -2616,22 +2616,22 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>TeClas Lives</t>
+          <t>Silvio Almeida</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TeClasLives</t>
+          <t>https://www.youtube.com/@silviolual</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Canal repositorio de Lives dos membros do canal Tecnologia e Classe</t>
+          <t>Sejam bem vindos ao meu canal!Uma voz ativa e relevante, que ja marca presenca nas redes sociais.Pode chegar que aqui nos vamos falar de assuntos densos atra...</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>UCu6wZb4i6D-C3huatVBUIFA</t>
+          <t>UCW3nde-8K-5BaHAmQLZ7ycg</t>
         </is>
       </c>
     </row>
@@ -2641,22 +2641,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Tecnologia e Classe</t>
+          <t>Soberana</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TecnologiaeClasse</t>
+          <t>https://www.youtube.com/@Soberana_TV</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t xml:space="preserve">TeClas e um canal sobre tecnologia e luta de classes, digitado pelos camaradas @azhariel.tv @lsaporiti @tresgatosnumjaleco e @lfzawacki </t>
+          <t>Bem vindo(a) a Soberana!Somos um coletivo de criadores marxistas-leninistas dedicados a producao de conteudo para a internet. Nosso objetivo e ocupar a inter...</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>UCYVrkMZdrjq5eICOG6Rxiwg</t>
+          <t>UC8tnKW-FN6LdvKazw5RmOOQ</t>
         </is>
       </c>
     </row>
@@ -2666,22 +2666,22 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Tempero Drag</t>
+          <t>Socialism For All / S4A ☭ Intensify Class Struggle</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TemperoDrag</t>
+          <t>https://www.youtube.com/@SocialismForAll</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Desde 2015 tratamos de temas sociais e politicos com humor e arte.Acreditamos na educacao como ferramenta de emancipacao e trabalhamos em uniao por mais e me...</t>
+          <t>I'm a US American studying Marxism (anti-revisionist Marxism-Leninism).I often post human-read audiobooks of socialist texts, &amp; I organize them into playlist...</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>UCZdJE8KpuFm6NRafHTEIC-g</t>
+          <t>UC5GYwuvmAD_VyV6w5aFnnUw</t>
         </is>
       </c>
     </row>
@@ -2691,22 +2691,22 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Tese Onze</t>
+          <t>Spooky Scary Socialist</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TeseOnze</t>
+          <t>https://www.youtube.com/@SpookyScarySocialist</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>O Tese Onze e um canal focado em apresentar contrapontos ao senso comum, trazer analises sobre sociologia e politica, e acumular bagagem pra transformar o mu...</t>
+          <t>eCommunist Homo~Animator</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>UC0fGGprihDIlQ3ykWvcb9hg</t>
+          <t>UCl_A_42M6kvjH8Gr-rwfCUw</t>
         </is>
       </c>
     </row>
@@ -2716,22 +2716,22 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>The Marxist Project</t>
+          <t>TV Boitempo</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@themarxistproject</t>
+          <t>https://www.youtube.com/@TVBoitempo</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Canal de videos da maior editora do pensamento critico da lingua portuguesa, com catalogo consistente reconhecido por sua qualidade e clareza de opcoes edito...</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>UCNalGyK3DaK37GTLIHSwmyA</t>
+          <t>UCzwfw0utuEVxc4D6ggXcqiQ</t>
         </is>
       </c>
     </row>
@@ -2741,22 +2741,22 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>The Peace Report</t>
+          <t>TV Grabois</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@ThePeaceReport</t>
+          <t>https://www.youtube.com/@TVGrabois</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+          <t>Espaco do pensamento marxista e progressista</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>UC9BpQd-PJNr_R2iyToRnoww</t>
+          <t>UCQ83chf0Yg1yt5Hrya1uVWQ</t>
         </is>
       </c>
     </row>
@@ -2766,22 +2766,22 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>TheFinnishBolshevik</t>
+          <t>TeClas Lives</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@thefinnishbolshevik2404</t>
+          <t>https://www.youtube.com/@TeClasLives</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>I'm a young Finnish Communist &amp; Marxist-Leninist.This channel is about the science of Marxism-Leninism. I give information and my personal thoughts on variou...</t>
+          <t>Canal repositorio de Lives dos membros do canal Tecnologia e Classe</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>UCCvdjsJtifsZoShjcAAHZpA</t>
+          <t>UCu6wZb4i6D-C3huatVBUIFA</t>
         </is>
       </c>
     </row>
@@ -2791,22 +2791,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Thiago Ávila - Bem Vivendo</t>
+          <t>Tecnologia e Classe</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@BemVivendo</t>
+          <t>https://www.youtube.com/@TecnologiaeClasse</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Um espaco criado para auxiliar na transformacao do mundo em um lugar mais justo, mais igualitario, em harmonia entre humanidade e natureza e com o Bem Viver ...</t>
+          <t xml:space="preserve">TeClas e um canal sobre tecnologia e luta de classes, digitado pelos camaradas @azhariel.tv @lsaporiti @tresgatosnumjaleco e @lfzawacki </t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>UCoAcADzxpCN6yot4MC0Az5A</t>
+          <t>UCYVrkMZdrjq5eICOG6Rxiwg</t>
         </is>
       </c>
     </row>
@@ -2816,22 +2816,22 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Tiago Andre Show!</t>
+          <t>Tempero Drag</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@tiagoandreshow</t>
+          <t>https://www.youtube.com/@TemperoDrag</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Sejam bem-vindos, seus lerdo, ao Tiago Andre Show!O Talk Show mais aleatorio e maluco ja existente e comandado por Tiago Santineli e seus pessimos funcionari...</t>
+          <t>Desde 2015 tratamos de temas sociais e politicos com humor e arte.Acreditamos na educacao como ferramenta de emancipacao e trabalhamos em uniao por mais e me...</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>UCIsJwHCdxmeM7APO-QIoj1A</t>
+          <t>UCZdJE8KpuFm6NRafHTEIC-g</t>
         </is>
       </c>
     </row>
@@ -2841,22 +2841,22 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Tiago Santineli</t>
+          <t>Tese Onze</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@TiagoSantineli</t>
+          <t>https://www.youtube.com/@TeseOnze</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>So se inscreve ai e pronto carai.</t>
+          <t>O Tese Onze e um canal focado em apresentar contrapontos ao senso comum, trazer analises sobre sociologia e politica, e acumular bagagem pra transformar o mu...</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>UCQimGgtBQmF4zxOdnARWFpg</t>
+          <t>UC0fGGprihDIlQ3ykWvcb9hg</t>
         </is>
       </c>
     </row>
@@ -2866,22 +2866,22 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Unlearning Economics</t>
+          <t>The Marxist Project</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@unlearningeconomics9021</t>
+          <t>https://www.youtube.com/@themarxistproject</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>I am an academic economist from the UK who has long been critical of the economics profession and how economics is used in public policy. Mostly the channel ...</t>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>UC4V_jMdRbbTrmBVJB6FDzgw</t>
+          <t>UCNalGyK3DaK37GTLIHSwmyA</t>
         </is>
       </c>
     </row>
@@ -2891,12 +2891,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Victor Camejo</t>
+          <t>The Peace Report</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@VictorCamejo</t>
+          <t>https://www.youtube.com/@ThePeaceReport</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>UCPHCzrKcFbS6gayKER3aNZw</t>
+          <t>UC9BpQd-PJNr_R2iyToRnoww</t>
         </is>
       </c>
     </row>
@@ -2916,22 +2916,22 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Wari'u</t>
+          <t>TheFinnishBolshevik</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>https://youtube.com/@wariu</t>
+          <t>https://www.youtube.com/@thefinnishbolshevik2404</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@wariu.com</t>
+          <t>I'm a young Finnish Communist &amp; Marxist-Leninist.This channel is about the science of Marxism-Leninism. I give information and my personal thoughts on variou...</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>UCZFj_5-VLQRddUKouwCSpbA</t>
+          <t>UCCvdjsJtifsZoShjcAAHZpA</t>
         </is>
       </c>
     </row>
@@ -2941,22 +2941,22 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>YUGOPNIK</t>
+          <t>Thiago Ávila - Bem Vivendo</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@YUGOPNIK</t>
+          <t>https://www.youtube.com/@BemVivendo</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>A Balkan Marx enthusaistTwitter: https://twitter.com/yugopnikEmail: Yugopnik@gmail.com</t>
+          <t>Um espaco criado para auxiliar na transformacao do mundo em um lugar mais justo, mais igualitario, em harmonia entre humanidade e natureza e com o Bem Viver ...</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>UCs8mbJ-M142ZskR5VR0gBig</t>
+          <t>UCoAcADzxpCN6yot4MC0Az5A</t>
         </is>
       </c>
     </row>
@@ -2966,22 +2966,22 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Zoe Baker</t>
+          <t>Tiago Andre Show!</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@anarchozoe</t>
+          <t>https://www.youtube.com/@tiagoandreshow</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>I'm a trans woman (she/her), who talks about the theory and history of anarchism, feminism and marxism. Author of Means and Ends: The Revolutionary Practice ...</t>
+          <t>Sejam bem-vindos, seus lerdo, ao Tiago Andre Show!O Talk Show mais aleatorio e maluco ja existente e comandado por Tiago Santineli e seus pessimos funcionari...</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>UC3FD64RRsrCLpiZNkq7ZkSg</t>
+          <t>UCIsJwHCdxmeM7APO-QIoj1A</t>
         </is>
       </c>
     </row>
@@ -2991,22 +2991,22 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>luideverso</t>
+          <t>Tiago Santineli</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@luideverso</t>
+          <t>https://www.youtube.com/@TiagoSantineli</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Ola, bem vindo ao canal de CORTES DO LUIDEVERSO. Me chamo Luide Matos e produzo conteudo ha 16 anos.Algumas informacoes importantes:- E um canal de react, so...</t>
+          <t>So se inscreve ai e pronto carai.</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>UCETjsiWHrAHyADOih7ACwHw</t>
+          <t>UCQimGgtBQmF4zxOdnARWFpg</t>
         </is>
       </c>
     </row>
@@ -3016,22 +3016,222 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
+          <t>Unlearning Economics</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@unlearningeconomics9021</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>I am an academic economist from the UK who has long been critical of the economics profession and how economics is used in public policy. Mostly the channel ...</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>UC4V_jMdRbbTrmBVJB6FDzgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Victor Camejo</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@VictorCamejo</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>UCPHCzrKcFbS6gayKER3aNZw</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>VinnyDays</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@ViniDays</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Canal de psicologo, psicanalista e produtor de conteudo marxista-leninista!Seja bem vindo, puxa uma cadeira e abre uma latinha que o papo vai comecar!Eu prod...</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>UCeC17rMD8Fhjwjt0yNjH8Xg</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Wari'u</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@wariu</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> contato@wariu.com</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>UCZFj_5-VLQRddUKouwCSpbA</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>YUGOPNIK</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@YUGOPNIK</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>A Balkan Marx enthusaistTwitter: https://twitter.com/yugopnikEmail: Yugopnik@gmail.com</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>UCs8mbJ-M142ZskR5VR0gBig</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Zoe Baker</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@anarchozoe</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>I'm a trans woman (she/her), who talks about the theory and history of anarchism, feminism and marxism. Author of Means and Ends: The Revolutionary Practice ...</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>UC3FD64RRsrCLpiZNkq7ZkSg</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>luideverso</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@luideverso</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Ola, bem vindo ao canal de CORTES DO LUIDEVERSO. Me chamo Luide Matos e produzo conteudo ha 16 anos.Algumas informacoes importantes:- E um canal de react, so...</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>UCETjsiWHrAHyADOih7ACwHw</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
           <t>münecat</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="C111" t="inlineStr">
         <is>
           <t>https://www.youtube.com/@munecat</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr">
+      <c r="D111" t="inlineStr">
         <is>
           <t>Compartilhe seus videos com amigos, familiares e todo o mundo</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
+      <c r="E111" t="inlineStr">
         <is>
           <t>UCqNpjt_UcMPgm_9gphZgHYA</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>oalgoritmodaimagem</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/@oalgoritmodaimagem</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Analises semioticas e sociologicas sobre celebridades, politicos e empresas.</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>UC2D8M-1psiJWfxj-aTe8pQA</t>
         </is>
       </c>
     </row>

</xml_diff>